<commit_message>
Generalized comparison algorithm, introduced
-- Adesso e' possibile inserire dei campi appositi nel file di esempio
"Amc_examples_data_xxx.xlsx" per far si che lo script "AMC_multipar.m"
faccia automaticamente il confronto tra il miglior candidato secondo
matlab e il miglio candidato secondo il VTM.

-- E' stato inserito il file "matlab_examples-summary.xlsx" che raccoglie tutti
gli esempi specificando se sono compliant con il VQ_Analyzer. In caso negativo,
riporta i dati che vengono fuori dal conforonto tra il candidato di Matlab e il candidato
del VTM.
</commit_message>
<xml_diff>
--- a/AMC_examples_data/AMC_examples_data_ex9.xlsx
+++ b/AMC_examples_data/AMC_examples_data_ex9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\5.2\Tesi\git\AMC_Model\AMC_examples_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A38C1A6-7D57-4BB9-AE69-72B591ECCF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A742CF62-BF6D-4656-B812-0FD5737A470C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFF8BB56-E23A-426B-9D6C-DA86724C81B1}"/>
+    <workbookView xWindow="-20610" yWindow="7980" windowWidth="20730" windowHeight="11160" xr2:uid="{FFF8BB56-E23A-426B-9D6C-DA86724C81B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>frame_h</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>.\sources\VQ_sample_432x240_Coded_8bit.yuv</t>
+  </si>
+  <si>
+    <t>VQ_best</t>
+  </si>
+  <si>
+    <t>comp_offs_x</t>
+  </si>
+  <si>
+    <t>comp_offs_y</t>
   </si>
 </sst>
 </file>
@@ -446,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F28914-79CE-4C5A-92B2-E41C9BEF8F7E}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,9 +468,12 @@
     <col min="10" max="10" width="13.85546875" customWidth="1"/>
     <col min="11" max="11" width="41.7109375" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="20" max="20" width="13" customWidth="1"/>
+    <col min="21" max="21" width="14.85546875" customWidth="1"/>
+    <col min="22" max="22" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -516,8 +528,17 @@
       <c r="S1" t="s">
         <v>17</v>
       </c>
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -575,8 +596,17 @@
       <c r="S2">
         <v>1</v>
       </c>
+      <c r="T2">
+        <v>2</v>
+      </c>
+      <c r="U2">
+        <v>89</v>
+      </c>
+      <c r="V2">
+        <v>203</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -598,8 +628,14 @@
       <c r="R3">
         <v>16</v>
       </c>
+      <c r="U3">
+        <v>88</v>
+      </c>
+      <c r="V3">
+        <v>204</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -622,12 +658,12 @@
         <v>-32</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>